<commit_message>
Updated documents for new test cases in s2.
</commit_message>
<xml_diff>
--- a/daffodil/sub-projects/core/doc/Test_Cases.xlsx
+++ b/daffodil/sub-projects/core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="27795" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Test Case ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="50">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -40,6 +37,135 @@
   </si>
   <si>
     <t xml:space="preserve">JIRA Issue Number </t>
+  </si>
+  <si>
+    <t>Test Case ID (Optional)</t>
+  </si>
+  <si>
+    <t>Long1</t>
+  </si>
+  <si>
+    <t>DFDL-5-012R</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>schema_types_5_04</t>
+  </si>
+  <si>
+    <t>BigInteger1</t>
+  </si>
+  <si>
+    <t>DFDL-5-011R</t>
+  </si>
+  <si>
+    <t>Integer01</t>
+  </si>
+  <si>
+    <t>Int01</t>
+  </si>
+  <si>
+    <t>DFDL-5-013R</t>
+  </si>
+  <si>
+    <t>schema_types_5_03</t>
+  </si>
+  <si>
+    <t>int_error</t>
+  </si>
+  <si>
+    <t>schema_types_5_02</t>
+  </si>
+  <si>
+    <t>DFDL-5-014R</t>
+  </si>
+  <si>
+    <t>UnsignedNumbers1</t>
+  </si>
+  <si>
+    <t>DFDL-5-017R</t>
+  </si>
+  <si>
+    <t>warning_exercise</t>
+  </si>
+  <si>
+    <t>Negative Test?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>DFDL-2-012R</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>unsignedLong_01</t>
+  </si>
+  <si>
+    <t>DFDL-88</t>
+  </si>
+  <si>
+    <t>DFDL-184</t>
+  </si>
+  <si>
+    <t>DFDL-185</t>
+  </si>
+  <si>
+    <t>DFDL-90</t>
+  </si>
+  <si>
+    <t>DFDL-210</t>
+  </si>
+  <si>
+    <t>unsignedLong_02</t>
+  </si>
+  <si>
+    <t>unsignedLong_03</t>
+  </si>
+  <si>
+    <t>Long2</t>
+  </si>
+  <si>
+    <t>short_01</t>
+  </si>
+  <si>
+    <t>unsignedInt_01</t>
+  </si>
+  <si>
+    <t>DFDL-5-018R</t>
+  </si>
+  <si>
+    <t>unsignedShort_01</t>
+  </si>
+  <si>
+    <t>DFDL-5-019R</t>
+  </si>
+  <si>
+    <t>unsignedByte_01</t>
+  </si>
+  <si>
+    <t>DFDL-5-020R</t>
+  </si>
+  <si>
+    <t>testRegEx_01</t>
+  </si>
+  <si>
+    <t>testRegEx_02</t>
+  </si>
+  <si>
+    <t>DFDL-24-002R</t>
+  </si>
+  <si>
+    <t>DFDL-216</t>
+  </si>
+  <si>
+    <t>int_error_02</t>
   </si>
 </sst>
 </file>
@@ -91,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -101,6 +227,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,48 +531,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test results and updated spreadsheets for new tests in spin 3.  Updated test descriptions with requirement ids.
</commit_message>
<xml_diff>
--- a/daffodil/sub-projects/core/doc/Test_Cases.xlsx
+++ b/daffodil/sub-projects/core/doc/Test_Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="104">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -166,6 +166,168 @@
   </si>
   <si>
     <t>int_error_02</t>
+  </si>
+  <si>
+    <t>length_delimited_12_02</t>
+  </si>
+  <si>
+    <t>DFDL-12-043R</t>
+  </si>
+  <si>
+    <t>DFDL-112</t>
+  </si>
+  <si>
+    <t>length_delimited_12_03</t>
+  </si>
+  <si>
+    <t>introduction_1_02</t>
+  </si>
+  <si>
+    <t>multiple_delimiters</t>
+  </si>
+  <si>
+    <t>DFDL-12-033R</t>
+  </si>
+  <si>
+    <t>NumSeq_01</t>
+  </si>
+  <si>
+    <t>DFDL-12-048R</t>
+  </si>
+  <si>
+    <t>NumSeq_03</t>
+  </si>
+  <si>
+    <t>DFDL-12-045R</t>
+  </si>
+  <si>
+    <t>DFDL-12-042R</t>
+  </si>
+  <si>
+    <t>NumSeq_04</t>
+  </si>
+  <si>
+    <t>AB000</t>
+  </si>
+  <si>
+    <t>AB001</t>
+  </si>
+  <si>
+    <t>AB002</t>
+  </si>
+  <si>
+    <t>AB003</t>
+  </si>
+  <si>
+    <t>AN000</t>
+  </si>
+  <si>
+    <t>AN001</t>
+  </si>
+  <si>
+    <t>AI000_rev</t>
+  </si>
+  <si>
+    <t>LengthKindPattern</t>
+  </si>
+  <si>
+    <t>DFDL-12-087R</t>
+  </si>
+  <si>
+    <t>DFDL-205</t>
+  </si>
+  <si>
+    <t>DFDL-12-088R</t>
+  </si>
+  <si>
+    <t>DFDL-207</t>
+  </si>
+  <si>
+    <t>LengthKindPatternCompound</t>
+  </si>
+  <si>
+    <t>lengthKindPattern_01</t>
+  </si>
+  <si>
+    <t>lengthKindPattern_02</t>
+  </si>
+  <si>
+    <t>lengthKindPattern_03</t>
+  </si>
+  <si>
+    <t>litNil1</t>
+  </si>
+  <si>
+    <t>DFDL-13-234R</t>
+  </si>
+  <si>
+    <t>DFDL-199</t>
+  </si>
+  <si>
+    <t>litNil2</t>
+  </si>
+  <si>
+    <t>multiple_delimiters2</t>
+  </si>
+  <si>
+    <t>DFDL-14-008R</t>
+  </si>
+  <si>
+    <t>DFDL-109</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>DFDL-204</t>
+  </si>
+  <si>
+    <t>choice2</t>
+  </si>
+  <si>
+    <t>DFDL-15-001R</t>
+  </si>
+  <si>
+    <t>choice3</t>
+  </si>
+  <si>
+    <t>choice4</t>
+  </si>
+  <si>
+    <t>choice5</t>
+  </si>
+  <si>
+    <t>choice6</t>
+  </si>
+  <si>
+    <t>choiceFail1</t>
+  </si>
+  <si>
+    <t>choiceDelim1</t>
+  </si>
+  <si>
+    <t>nestedChoice1</t>
+  </si>
+  <si>
+    <t>property_scoping_01</t>
+  </si>
+  <si>
+    <t>DFDL-8-009R</t>
+  </si>
+  <si>
+    <t>DFDL-224</t>
+  </si>
+  <si>
+    <t>syntax_entities_6_02</t>
+  </si>
+  <si>
+    <t>DFDL-6-042R</t>
+  </si>
+  <si>
+    <t>DFDL-219</t>
+  </si>
+  <si>
+    <t>byte</t>
   </si>
 </sst>
 </file>
@@ -531,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,6 +1255,768 @@
       </c>
       <c r="I22" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="5">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="5">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="5">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="5">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="5">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="5">
+        <v>3</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="5">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="5">
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="5">
+        <v>3</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="5">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="5">
+        <v>3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="5">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="5">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="5">
+        <v>3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="5">
+        <v>3</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="5">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="5">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="5">
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>87</v>
+      </c>
+      <c r="I51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="5">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="5">
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="5">
+        <v>3</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="5">
+        <v>3</v>
+      </c>
+      <c r="G55" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1126,6 +2050,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D82A129E61AB94CBD557DF296383A78" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8177165d1a918059be1ae03aa3b2f972">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1174,15 +2107,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -1190,6 +2114,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EBC05A-E30D-4C65-8413-46397881E931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1204,24 +2136,16 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A2441A-1352-406E-94CB-A261B0FDC5B0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated spreadsheets with new tests from spin 3
</commit_message>
<xml_diff>
--- a/daffodil/sub-projects/core/doc/Test_Cases.xlsx
+++ b/daffodil/sub-projects/core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="27795" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="27795" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="134">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -328,6 +328,96 @@
   </si>
   <si>
     <t>byte</t>
+  </si>
+  <si>
+    <t>schema_types_5_01</t>
+  </si>
+  <si>
+    <t>DFDL-5-015R</t>
+  </si>
+  <si>
+    <t>schema_types_5_05</t>
+  </si>
+  <si>
+    <t>syntax_entities_6_01</t>
+  </si>
+  <si>
+    <t>DFDL-6-041R</t>
+  </si>
+  <si>
+    <t>syntax_entities_6_03</t>
+  </si>
+  <si>
+    <t>DFDL-6-045R</t>
+  </si>
+  <si>
+    <t>NextLine</t>
+  </si>
+  <si>
+    <t>LineSeparator</t>
+  </si>
+  <si>
+    <t>LineFeed</t>
+  </si>
+  <si>
+    <t>CarriageReturn</t>
+  </si>
+  <si>
+    <t>FormFeed</t>
+  </si>
+  <si>
+    <t>CarriageReturn_byte</t>
+  </si>
+  <si>
+    <t>DFDL-141</t>
+  </si>
+  <si>
+    <t>LineFeed_byte</t>
+  </si>
+  <si>
+    <t>LineSeparator_byte</t>
+  </si>
+  <si>
+    <t>NextLine_byte</t>
+  </si>
+  <si>
+    <t>CRLF_byte</t>
+  </si>
+  <si>
+    <t>lengthKindDelimited_01</t>
+  </si>
+  <si>
+    <t>lengthKindDelimited_02</t>
+  </si>
+  <si>
+    <t>DFDL-142</t>
+  </si>
+  <si>
+    <t>DFDL-12-032R</t>
+  </si>
+  <si>
+    <t>delimiter_12_03</t>
+  </si>
+  <si>
+    <t>SeqGrp_01</t>
+  </si>
+  <si>
+    <t>litNil3</t>
+  </si>
+  <si>
+    <t>DFDL-13-236R</t>
+  </si>
+  <si>
+    <t>DelimProp_01</t>
+  </si>
+  <si>
+    <t>DFDL-203</t>
+  </si>
+  <si>
+    <t>ParseSequence4</t>
+  </si>
+  <si>
+    <t>ParseSequence5</t>
   </si>
 </sst>
 </file>
@@ -693,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,6 +2107,512 @@
       </c>
       <c r="H55" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="5">
+        <v>3</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="5">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="5">
+        <v>3</v>
+      </c>
+      <c r="G58" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="5">
+        <v>3</v>
+      </c>
+      <c r="G59" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="5">
+        <v>3</v>
+      </c>
+      <c r="G60" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="5">
+        <v>3</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" t="s">
+        <v>110</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="5">
+        <v>3</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="5">
+        <v>3</v>
+      </c>
+      <c r="G63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="5">
+        <v>3</v>
+      </c>
+      <c r="G64" t="s">
+        <v>103</v>
+      </c>
+      <c r="H64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" t="s">
+        <v>110</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="5">
+        <v>3</v>
+      </c>
+      <c r="G65" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="5">
+        <v>3</v>
+      </c>
+      <c r="G66" t="s">
+        <v>103</v>
+      </c>
+      <c r="H66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="5">
+        <v>3</v>
+      </c>
+      <c r="G67" t="s">
+        <v>103</v>
+      </c>
+      <c r="H67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" t="s">
+        <v>110</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="5">
+        <v>3</v>
+      </c>
+      <c r="G68" t="s">
+        <v>103</v>
+      </c>
+      <c r="H68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="5">
+        <v>3</v>
+      </c>
+      <c r="G69" t="s">
+        <v>103</v>
+      </c>
+      <c r="H69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
+        <v>58</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="5">
+        <v>3</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="5">
+        <v>3</v>
+      </c>
+      <c r="G71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" t="s">
+        <v>125</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="5">
+        <v>3</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D73" t="s">
+        <v>84</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="5">
+        <v>3</v>
+      </c>
+      <c r="G73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="5">
+        <v>3</v>
+      </c>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>130</v>
+      </c>
+      <c r="C75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" t="s">
+        <v>125</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="5">
+        <v>3</v>
+      </c>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D76" t="s">
+        <v>125</v>
+      </c>
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="5">
+        <v>3</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>133</v>
+      </c>
+      <c r="C77" t="s">
+        <v>28</v>
+      </c>
+      <c r="D77" t="s">
+        <v>125</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="5">
+        <v>3</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>